<commit_message>
Update:"Thay trường email bằng ngày sinh"
</commit_message>
<xml_diff>
--- a/source code/front-end-user/src/assets/excel/user-import-template.xlsx
+++ b/source code/front-end-user/src/assets/excel/user-import-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\DuAn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LinhTinh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A7EC867-4DEE-4B44-A945-ECB74376C908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4139DA2E-64C4-45F3-9AAA-10BD634A7344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{960549A1-3B70-4FCE-BCF9-93BB2D766178}"/>
+    <workbookView xWindow="3564" yWindow="2760" windowWidth="17280" windowHeight="8880" xr2:uid="{E1AB712F-2108-4148-98B8-60DA86615350}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,69 +36,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Intake Code</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>student01</t>
-  </si>
-  <si>
-    <t>student01@example.com</t>
-  </si>
-  <si>
-    <t>An</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+  <si>
+    <t>Tên đăng nhập</t>
+  </si>
+  <si>
+    <t>Mật khẩu</t>
+  </si>
+  <si>
+    <t>Họ</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>Mã lớp (intake)</t>
+  </si>
+  <si>
+    <t>Vai trò</t>
+  </si>
+  <si>
+    <t>tuan01</t>
   </si>
   <si>
     <t>Nguyen</t>
   </si>
   <si>
+    <t>Tuan</t>
+  </si>
+  <si>
     <t>STUDENT</t>
   </si>
   <si>
-    <t>admin01</t>
-  </si>
-  <si>
-    <t>admin01@example.com</t>
-  </si>
-  <si>
-    <t>Linh</t>
+    <t>admin02</t>
+  </si>
+  <si>
+    <t>Tran</t>
+  </si>
+  <si>
+    <t>Hanh</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>teacher01</t>
   </si>
   <si>
     <t>Pham</t>
   </si>
   <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>lecturer01</t>
-  </si>
-  <si>
-    <t>lecturer01@example.com</t>
-  </si>
-  <si>
-    <t>Bao</t>
-  </si>
-  <si>
-    <t>Tran</t>
+    <t>Hai</t>
   </si>
   <si>
     <t>LECTURER</t>
@@ -111,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,12 +119,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,11 +141,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -165,12 +152,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,25 +491,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D65999-77AD-4068-81B2-B823C99929DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4928CAD0-C081-472F-BE21-9EB59334ED78}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,77 +526,72 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="26.4">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4">
+        <v>38698</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4">
+        <v>36651</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
+    <row r="4" spans="1:7" ht="26.4">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="4">
+        <v>32331</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:student01@example.com" xr:uid="{55588DB1-2D23-43AB-90C3-A65999E2CF61}"/>
-    <hyperlink ref="C3" r:id="rId2" display="mailto:admin01@example.com" xr:uid="{BAC643AA-7202-4CA7-97C7-D2964FBDE9BB}"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:lecturer01@example.com" xr:uid="{8B27E0CE-2974-49C4-A4CB-AE3E1440C5CD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>